<commit_message>
Add link to detail in User/_Profile.cshtml
</commit_message>
<xml_diff>
--- a/WIP/Documents/Report 3/WS_Integration Test Case_v1.0_EN.xlsx
+++ b/WIP/Documents/Report 3/WS_Integration Test Case_v1.0_EN.xlsx
@@ -18,9 +18,10 @@
     <sheet name="Message Rules" sheetId="11" r:id="rId4"/>
     <sheet name="User_Function" sheetId="9" r:id="rId5"/>
     <sheet name="Admin_Function" sheetId="10" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="12" state="hidden" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="ACTION" localSheetId="3">#REF!</definedName>
@@ -32,6 +33,7 @@
     <definedName name="Lỗi">#REF!</definedName>
     <definedName name="Pass">#REF!</definedName>
     <definedName name="Statistic" comment="fsfsdfs">#REF!</definedName>
+    <definedName name="TestList">Sheet1!$A$2:$A$6</definedName>
   </definedNames>
   <calcPr calcId="152511" iterate="1" iterateCount="10000" iterateDelta="1.0000000000000001E-5"/>
 </workbook>
@@ -200,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="723">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -2057,12 +2059,6 @@
     <t>Edit Thread with delete all data in not-require field</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Go to wings.com
-2. Login with available account
-3. Click on "Thông tin tài khoản" -&gt; "Thảo luận"
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.The Homepage is displayed 
 2. Go to user homepage
 3. Created thread page displayed and status is Active
@@ -2072,14 +2068,6 @@
     <t xml:space="preserve">1.The Homepage is displayed 
 2. Go to user homepage
 3. Created thread page displayed and status is De-Active
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Go to wings.com
-2. Login with available account
-3. Click on "Thông tin tài khoản" -&gt; "Thảo luận"
-4. Click Edit
-5. Do no change data and click save
 </t>
   </si>
   <si>
@@ -3402,6 +3390,35 @@
 4. All input are displayed
 5. Create Organization successful and display waiting approve notice
 6. Recive emai accept from Admin
+</t>
+  </si>
+  <si>
+    <t>Untest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Go to wings.com
+2. Login with available account
+3. Click on "Thông tin tài khoản" -&gt; "Bài viết đã tạo"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.The Homepage is displayed 
+2. Go to user homepage
+3. Created thread tab displayed and status is Active
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.The Homepage is displayed 
+2. Go to user homepage
+3. Created thread tab displayed and status is De-Active
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Go to wings.com
+2. Login with available account
+3. Click on "Thông tin tài khoản" -&gt; "Bài viết đã tạo"
+4. Click Edit
+5. Do no change data and click save
 </t>
   </si>
 </sst>
@@ -6259,7 +6276,7 @@
       </c>
       <c r="D11" s="76">
         <f>User_Function!A6</f>
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="E11" s="76">
         <f>User_Function!B6</f>
@@ -6267,7 +6284,7 @@
       </c>
       <c r="F11" s="76">
         <f>User_Function!C6</f>
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="G11" s="76">
         <f>User_Function!D6</f>
@@ -6315,7 +6332,7 @@
       </c>
       <c r="D13" s="79">
         <f>SUM(D9:D12)</f>
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="E13" s="79">
         <f>SUM(E9:E12)</f>
@@ -6323,7 +6340,7 @@
       </c>
       <c r="F13" s="79">
         <f>SUM(F9:F12)</f>
-        <v>288</v>
+        <v>264</v>
       </c>
       <c r="G13" s="79">
         <f>SUM(G9:G12)</f>
@@ -6353,7 +6370,7 @@
       <c r="D15" s="70"/>
       <c r="E15" s="85">
         <f>(D13+E13)*100/(H13-G13)</f>
-        <v>34.841628959276015</v>
+        <v>40.271493212669682</v>
       </c>
       <c r="F15" s="70" t="s">
         <v>43</v>
@@ -6370,7 +6387,7 @@
       <c r="D16" s="70"/>
       <c r="E16" s="85">
         <f>D13*100/(H13-G13)</f>
-        <v>33.0316742081448</v>
+        <v>38.46153846153846</v>
       </c>
       <c r="F16" s="70" t="s">
         <v>43</v>
@@ -6680,7 +6697,7 @@
         <v>109</v>
       </c>
       <c r="B30" s="161" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C30" s="161"/>
     </row>
@@ -6689,7 +6706,7 @@
         <v>110</v>
       </c>
       <c r="B31" s="161" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C31" s="161"/>
     </row>
@@ -6727,8 +6744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.25" defaultRowHeight="13.5" customHeight="1"/>
@@ -8024,7 +8041,7 @@
     <row r="6" spans="1:252" ht="13.5" customHeight="1" thickBot="1">
       <c r="A6" s="130">
         <f>COUNTIF(F11:G340,"Pass")</f>
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="B6" s="101">
         <f>COUNTIF(F11:G787,"Fail")</f>
@@ -8032,7 +8049,7 @@
       </c>
       <c r="C6" s="101">
         <f>E6-D6-B6-A6</f>
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="D6" s="102">
         <f>COUNTIF(F11:G787,"N/A")</f>
@@ -12159,10 +12176,10 @@
         <v>114</v>
       </c>
       <c r="B22" s="91" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="C22" s="91" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="D22" s="91" t="s">
         <v>264</v>
@@ -12420,13 +12437,13 @@
         <v>115</v>
       </c>
       <c r="B23" s="91" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C23" s="91" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="D23" s="91" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="E23" s="146"/>
       <c r="F23" s="117" t="s">
@@ -12681,13 +12698,13 @@
         <v>116</v>
       </c>
       <c r="B24" s="91" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C24" s="91" t="s">
+        <v>671</v>
+      </c>
+      <c r="D24" s="91" t="s">
         <v>673</v>
-      </c>
-      <c r="D24" s="91" t="s">
-        <v>675</v>
       </c>
       <c r="E24" s="146"/>
       <c r="F24" s="117" t="s">
@@ -12942,10 +12959,10 @@
         <v>117</v>
       </c>
       <c r="B25" s="91" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C25" s="91" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="D25" s="91" t="s">
         <v>359</v>
@@ -13203,10 +13220,10 @@
         <v>266</v>
       </c>
       <c r="B26" s="91" t="s">
+        <v>669</v>
+      </c>
+      <c r="C26" s="91" t="s">
         <v>671</v>
-      </c>
-      <c r="C26" s="91" t="s">
-        <v>673</v>
       </c>
       <c r="D26" s="91" t="s">
         <v>360</v>
@@ -13464,13 +13481,13 @@
         <v>267</v>
       </c>
       <c r="B27" s="91" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C27" s="91" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="D27" s="91" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="E27" s="146"/>
       <c r="F27" s="117" t="s">
@@ -13725,13 +13742,13 @@
         <v>268</v>
       </c>
       <c r="B28" s="91" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C28" s="91" t="s">
         <v>259</v>
       </c>
       <c r="D28" s="91" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="E28" s="146"/>
       <c r="F28" s="117" t="s">
@@ -13986,7 +14003,7 @@
         <v>269</v>
       </c>
       <c r="B29" s="91" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="C29" s="91" t="s">
         <v>259</v>
@@ -14247,7 +14264,7 @@
         <v>367</v>
       </c>
       <c r="B30" s="91" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="C30" s="91" t="s">
         <v>259</v>
@@ -14508,7 +14525,7 @@
         <v>368</v>
       </c>
       <c r="B31" s="91" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C31" s="91" t="s">
         <v>259</v>
@@ -14769,7 +14786,7 @@
         <v>369</v>
       </c>
       <c r="B32" s="91" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="C32" s="91" t="s">
         <v>260</v>
@@ -15030,13 +15047,13 @@
         <v>370</v>
       </c>
       <c r="B33" s="91" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C33" s="91" t="s">
         <v>260</v>
       </c>
       <c r="D33" s="91" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="E33" s="146"/>
       <c r="F33" s="117" t="s">
@@ -15291,7 +15308,7 @@
         <v>371</v>
       </c>
       <c r="B34" s="91" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C34" s="91" t="s">
         <v>260</v>
@@ -15552,7 +15569,7 @@
         <v>372</v>
       </c>
       <c r="B35" s="91" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C35" s="91" t="s">
         <v>260</v>
@@ -15813,7 +15830,7 @@
         <v>373</v>
       </c>
       <c r="B36" s="91" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="C36" s="91" t="s">
         <v>260</v>
@@ -16074,7 +16091,7 @@
         <v>374</v>
       </c>
       <c r="B37" s="91" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C37" s="91" t="s">
         <v>265</v>
@@ -16335,13 +16352,13 @@
         <v>375</v>
       </c>
       <c r="B38" s="91" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="C38" s="91" t="s">
         <v>265</v>
       </c>
       <c r="D38" s="91" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="E38" s="146"/>
       <c r="F38" s="117" t="s">
@@ -16596,7 +16613,7 @@
         <v>376</v>
       </c>
       <c r="B39" s="91" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C39" s="91" t="s">
         <v>364</v>
@@ -16857,7 +16874,7 @@
         <v>377</v>
       </c>
       <c r="B40" s="91" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="C40" s="91" t="s">
         <v>364</v>
@@ -17118,7 +17135,7 @@
         <v>378</v>
       </c>
       <c r="B41" s="91" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="C41" s="91" t="s">
         <v>364</v>
@@ -17379,7 +17396,7 @@
         <v>379</v>
       </c>
       <c r="B42" s="91" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="C42" s="91" t="s">
         <v>261</v>
@@ -17640,13 +17657,13 @@
         <v>380</v>
       </c>
       <c r="B43" s="91" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="C43" s="91" t="s">
         <v>365</v>
       </c>
       <c r="D43" s="91" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="E43" s="146"/>
       <c r="F43" s="117" t="s">
@@ -17901,7 +17918,7 @@
         <v>381</v>
       </c>
       <c r="B44" s="91" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="C44" s="91" t="s">
         <v>365</v>
@@ -18162,7 +18179,7 @@
         <v>382</v>
       </c>
       <c r="B45" s="91" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="C45" s="91" t="s">
         <v>365</v>
@@ -18423,7 +18440,7 @@
         <v>383</v>
       </c>
       <c r="B46" s="91" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C46" s="91" t="s">
         <v>365</v>
@@ -18684,7 +18701,7 @@
         <v>384</v>
       </c>
       <c r="B47" s="91" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="C47" s="91" t="s">
         <v>270</v>
@@ -18945,7 +18962,7 @@
         <v>385</v>
       </c>
       <c r="B48" s="91" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C48" s="91" t="s">
         <v>272</v>
@@ -19206,7 +19223,7 @@
         <v>386</v>
       </c>
       <c r="B49" s="91" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C49" s="91" t="s">
         <v>366</v>
@@ -19467,7 +19484,7 @@
         <v>387</v>
       </c>
       <c r="B50" s="91" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C50" s="91" t="s">
         <v>366</v>
@@ -24188,7 +24205,7 @@
         <v>241</v>
       </c>
       <c r="D68" s="136" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="E68" s="91"/>
       <c r="F68" s="117" t="s">
@@ -26849,10 +26866,10 @@
         <v>68</v>
       </c>
       <c r="C78" s="91" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="D78" s="91" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E78" s="91"/>
       <c r="F78" s="117" t="s">
@@ -28889,7 +28906,7 @@
     <row r="86" spans="1:245" ht="14.25" customHeight="1">
       <c r="A86" s="223"/>
       <c r="B86" s="223" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C86" s="224"/>
       <c r="D86" s="224"/>
@@ -28936,10 +28953,10 @@
         <v>285</v>
       </c>
       <c r="C88" s="106" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D88" s="104" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E88" s="167"/>
       <c r="F88" s="117" t="s">
@@ -28963,7 +28980,7 @@
         <v>389</v>
       </c>
       <c r="C89" s="106" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="D89" s="104" t="s">
         <v>390</v>
@@ -28990,7 +29007,7 @@
         <v>391</v>
       </c>
       <c r="C90" s="106" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="D90" s="104" t="s">
         <v>392</v>
@@ -29014,13 +29031,13 @@
         <v>[User_login-81]</v>
       </c>
       <c r="B91" s="91" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C91" s="106" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D91" s="104" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E91" s="167"/>
       <c r="F91" s="117" t="s">
@@ -29041,10 +29058,10 @@
         <v>[User_login-82]</v>
       </c>
       <c r="B92" s="91" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C92" s="106" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="D92" s="104" t="s">
         <v>392</v>
@@ -29068,13 +29085,13 @@
         <v>[User_login-83]</v>
       </c>
       <c r="B93" s="91" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C93" s="106" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D93" s="104" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="E93" s="167"/>
       <c r="F93" s="117" t="s">
@@ -29095,13 +29112,13 @@
         <v>[User_login-84]</v>
       </c>
       <c r="B94" s="91" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C94" s="106" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="D94" s="104" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E94" s="167"/>
       <c r="F94" s="117" t="s">
@@ -29253,7 +29270,7 @@
         <v>419</v>
       </c>
       <c r="D100" s="117" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="E100" s="163"/>
       <c r="F100" s="117" t="s">
@@ -29280,11 +29297,15 @@
         <v>421</v>
       </c>
       <c r="D101" s="117" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="E101" s="163"/>
-      <c r="F101" s="117"/>
-      <c r="G101" s="117"/>
+      <c r="F101" s="117" t="s">
+        <v>22</v>
+      </c>
+      <c r="G101" s="117" t="s">
+        <v>22</v>
+      </c>
       <c r="H101" s="112">
         <v>42412</v>
       </c>
@@ -29306,8 +29327,12 @@
         <v>426</v>
       </c>
       <c r="E102" s="163"/>
-      <c r="F102" s="117"/>
-      <c r="G102" s="117"/>
+      <c r="F102" s="117" t="s">
+        <v>22</v>
+      </c>
+      <c r="G102" s="117" t="s">
+        <v>22</v>
+      </c>
       <c r="H102" s="112">
         <v>42412</v>
       </c>
@@ -29329,8 +29354,12 @@
         <v>427</v>
       </c>
       <c r="E103" s="163"/>
-      <c r="F103" s="117"/>
-      <c r="G103" s="117"/>
+      <c r="F103" s="117" t="s">
+        <v>22</v>
+      </c>
+      <c r="G103" s="117" t="s">
+        <v>22</v>
+      </c>
       <c r="H103" s="112">
         <v>42412</v>
       </c>
@@ -29352,8 +29381,12 @@
         <v>430</v>
       </c>
       <c r="E104" s="163"/>
-      <c r="F104" s="117"/>
-      <c r="G104" s="117"/>
+      <c r="F104" s="117" t="s">
+        <v>22</v>
+      </c>
+      <c r="G104" s="117" t="s">
+        <v>22</v>
+      </c>
       <c r="H104" s="112">
         <v>42412</v>
       </c>
@@ -29375,8 +29408,12 @@
         <v>433</v>
       </c>
       <c r="E105" s="163"/>
-      <c r="F105" s="117"/>
-      <c r="G105" s="117"/>
+      <c r="F105" s="117" t="s">
+        <v>22</v>
+      </c>
+      <c r="G105" s="117" t="s">
+        <v>22</v>
+      </c>
       <c r="H105" s="112">
         <v>42412</v>
       </c>
@@ -29398,8 +29435,12 @@
         <v>436</v>
       </c>
       <c r="E106" s="163"/>
-      <c r="F106" s="117"/>
-      <c r="G106" s="117"/>
+      <c r="F106" s="117" t="s">
+        <v>22</v>
+      </c>
+      <c r="G106" s="117" t="s">
+        <v>22</v>
+      </c>
       <c r="H106" s="112">
         <v>42412</v>
       </c>
@@ -29421,8 +29462,12 @@
         <v>433</v>
       </c>
       <c r="E107" s="163"/>
-      <c r="F107" s="117"/>
-      <c r="G107" s="117"/>
+      <c r="F107" s="117" t="s">
+        <v>22</v>
+      </c>
+      <c r="G107" s="117" t="s">
+        <v>22</v>
+      </c>
       <c r="H107" s="112">
         <v>42412</v>
       </c>
@@ -29442,9 +29487,7 @@
       <c r="E108" s="231"/>
       <c r="F108" s="231"/>
       <c r="G108" s="231"/>
-      <c r="H108" s="112">
-        <v>42412</v>
-      </c>
+      <c r="H108" s="112"/>
       <c r="I108" s="231"/>
       <c r="J108" s="105"/>
     </row>
@@ -29463,8 +29506,12 @@
         <v>297</v>
       </c>
       <c r="E109" s="163"/>
-      <c r="F109" s="117"/>
-      <c r="G109" s="117"/>
+      <c r="F109" s="117" t="s">
+        <v>22</v>
+      </c>
+      <c r="G109" s="117" t="s">
+        <v>22</v>
+      </c>
       <c r="H109" s="112">
         <v>42412</v>
       </c>
@@ -29486,8 +29533,12 @@
         <v>298</v>
       </c>
       <c r="E110" s="163"/>
-      <c r="F110" s="117"/>
-      <c r="G110" s="117"/>
+      <c r="F110" s="117" t="s">
+        <v>22</v>
+      </c>
+      <c r="G110" s="117" t="s">
+        <v>22</v>
+      </c>
       <c r="H110" s="112">
         <v>42412</v>
       </c>
@@ -29509,8 +29560,12 @@
         <v>321</v>
       </c>
       <c r="E111" s="163"/>
-      <c r="F111" s="117"/>
-      <c r="G111" s="117"/>
+      <c r="F111" s="117" t="s">
+        <v>22</v>
+      </c>
+      <c r="G111" s="117" t="s">
+        <v>22</v>
+      </c>
       <c r="H111" s="112">
         <v>42412</v>
       </c>
@@ -29526,14 +29581,18 @@
         <v>440</v>
       </c>
       <c r="C112" s="166" t="s">
-        <v>446</v>
+        <v>719</v>
       </c>
       <c r="D112" s="117" t="s">
-        <v>447</v>
+        <v>720</v>
       </c>
       <c r="E112" s="163"/>
-      <c r="F112" s="117"/>
-      <c r="G112" s="117"/>
+      <c r="F112" s="117" t="s">
+        <v>22</v>
+      </c>
+      <c r="G112" s="117" t="s">
+        <v>22</v>
+      </c>
       <c r="H112" s="112">
         <v>42412</v>
       </c>
@@ -29549,14 +29608,18 @@
         <v>441</v>
       </c>
       <c r="C113" s="166" t="s">
-        <v>446</v>
+        <v>719</v>
       </c>
       <c r="D113" s="117" t="s">
-        <v>448</v>
+        <v>721</v>
       </c>
       <c r="E113" s="163"/>
-      <c r="F113" s="117"/>
-      <c r="G113" s="117"/>
+      <c r="F113" s="117" t="s">
+        <v>22</v>
+      </c>
+      <c r="G113" s="117" t="s">
+        <v>22</v>
+      </c>
       <c r="H113" s="112">
         <v>42412</v>
       </c>
@@ -29572,10 +29635,10 @@
         <v>442</v>
       </c>
       <c r="C114" s="166" t="s">
-        <v>449</v>
+        <v>722</v>
       </c>
       <c r="D114" s="117" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E114" s="163"/>
       <c r="F114" s="117"/>
@@ -29595,10 +29658,10 @@
         <v>443</v>
       </c>
       <c r="C115" s="166" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D115" s="117" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E115" s="163"/>
       <c r="F115" s="117"/>
@@ -29618,10 +29681,10 @@
         <v>444</v>
       </c>
       <c r="C116" s="166" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D116" s="117" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E116" s="163"/>
       <c r="F116" s="117"/>
@@ -29641,10 +29704,10 @@
         <v>445</v>
       </c>
       <c r="C117" s="166" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D117" s="117" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E117" s="163"/>
       <c r="F117" s="117"/>
@@ -29661,7 +29724,7 @@
         <v>[User_login-108]</v>
       </c>
       <c r="B118" s="223" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C118" s="231"/>
       <c r="D118" s="231"/>
@@ -29749,13 +29812,13 @@
         <v>[User_login-112]</v>
       </c>
       <c r="B122" s="175" t="s">
+        <v>455</v>
+      </c>
+      <c r="C122" s="166" t="s">
+        <v>456</v>
+      </c>
+      <c r="D122" s="117" t="s">
         <v>457</v>
-      </c>
-      <c r="C122" s="166" t="s">
-        <v>458</v>
-      </c>
-      <c r="D122" s="117" t="s">
-        <v>459</v>
       </c>
       <c r="E122" s="163"/>
       <c r="F122" s="117"/>
@@ -29772,13 +29835,13 @@
         <v>[User_login-113]</v>
       </c>
       <c r="B123" s="175" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C123" s="166" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D123" s="117" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E123" s="163"/>
       <c r="F123" s="117"/>
@@ -29795,13 +29858,13 @@
         <v>[User_login-114]</v>
       </c>
       <c r="B124" s="175" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C124" s="166" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D124" s="117" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E124" s="163"/>
       <c r="F124" s="117"/>
@@ -29818,13 +29881,13 @@
         <v>[User_login-115]</v>
       </c>
       <c r="B125" s="175" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C125" s="166" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D125" s="117" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E125" s="163"/>
       <c r="F125" s="117"/>
@@ -29841,13 +29904,13 @@
         <v>[User_login-116]</v>
       </c>
       <c r="B126" s="175" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C126" s="166" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D126" s="117" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="E126" s="163"/>
       <c r="F126" s="117"/>
@@ -29864,13 +29927,13 @@
         <v>[User_login-117]</v>
       </c>
       <c r="B127" s="175" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C127" s="166" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D127" s="117" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E127" s="163"/>
       <c r="F127" s="117"/>
@@ -29887,13 +29950,13 @@
         <v>[User_login-118]</v>
       </c>
       <c r="B128" s="175" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C128" s="166" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D128" s="117" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E128" s="163"/>
       <c r="F128" s="117"/>
@@ -29910,13 +29973,13 @@
         <v>[User_login-119]</v>
       </c>
       <c r="B129" s="175" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C129" s="166" t="s">
+        <v>472</v>
+      </c>
+      <c r="D129" s="117" t="s">
         <v>474</v>
-      </c>
-      <c r="D129" s="117" t="s">
-        <v>476</v>
       </c>
       <c r="E129" s="163"/>
       <c r="F129" s="117"/>
@@ -29933,7 +29996,7 @@
         <v>[User_login-120]</v>
       </c>
       <c r="B130" s="223" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C130" s="231"/>
       <c r="D130" s="231"/>
@@ -29952,13 +30015,13 @@
         <v>[User_login-121]</v>
       </c>
       <c r="B131" s="175" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C131" s="166" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D131" s="117" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E131" s="163"/>
       <c r="F131" s="117"/>
@@ -29975,13 +30038,13 @@
         <v>[User_login-122]</v>
       </c>
       <c r="B132" s="175" t="s">
+        <v>490</v>
+      </c>
+      <c r="C132" s="166" t="s">
         <v>492</v>
       </c>
-      <c r="C132" s="166" t="s">
-        <v>494</v>
-      </c>
       <c r="D132" s="117" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E132" s="163"/>
       <c r="F132" s="117"/>
@@ -29998,13 +30061,13 @@
         <v>[User_login-123]</v>
       </c>
       <c r="B133" s="117" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C133" s="117" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D133" s="117" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E133" s="163"/>
       <c r="F133" s="117"/>
@@ -30021,13 +30084,13 @@
         <v>[User_login-124]</v>
       </c>
       <c r="B134" s="117" t="s">
+        <v>493</v>
+      </c>
+      <c r="C134" s="117" t="s">
         <v>495</v>
       </c>
-      <c r="C134" s="117" t="s">
-        <v>497</v>
-      </c>
       <c r="D134" s="117" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E134" s="163"/>
       <c r="F134" s="117"/>
@@ -30044,13 +30107,13 @@
         <v>[User_login-125]</v>
       </c>
       <c r="B135" s="117" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C135" s="117" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D135" s="117" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E135" s="163"/>
       <c r="F135" s="117"/>
@@ -30065,13 +30128,13 @@
         <v>[User_login-126]</v>
       </c>
       <c r="B136" s="117" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C136" s="117" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D136" s="117" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E136" s="163"/>
       <c r="F136" s="117"/>
@@ -30086,13 +30149,13 @@
         <v>[User_login-127]</v>
       </c>
       <c r="B137" s="117" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C137" s="117" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D137" s="117" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E137" s="163"/>
       <c r="F137" s="117"/>
@@ -30107,13 +30170,13 @@
         <v>[User_login-128]</v>
       </c>
       <c r="B138" s="117" t="s">
+        <v>494</v>
+      </c>
+      <c r="C138" s="117" t="s">
+        <v>498</v>
+      </c>
+      <c r="D138" s="117" t="s">
         <v>496</v>
-      </c>
-      <c r="C138" s="117" t="s">
-        <v>500</v>
-      </c>
-      <c r="D138" s="117" t="s">
-        <v>498</v>
       </c>
       <c r="E138" s="163"/>
       <c r="F138" s="117"/>
@@ -30128,13 +30191,13 @@
         <v>[User_login-129]</v>
       </c>
       <c r="B139" s="117" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C139" s="117" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D139" s="117" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E139" s="163"/>
       <c r="F139" s="117"/>
@@ -30149,13 +30212,13 @@
         <v>[User_login-130]</v>
       </c>
       <c r="B140" s="117" t="s">
+        <v>505</v>
+      </c>
+      <c r="C140" s="117" t="s">
+        <v>506</v>
+      </c>
+      <c r="D140" s="117" t="s">
         <v>507</v>
-      </c>
-      <c r="C140" s="117" t="s">
-        <v>508</v>
-      </c>
-      <c r="D140" s="117" t="s">
-        <v>509</v>
       </c>
       <c r="E140" s="163"/>
       <c r="F140" s="117"/>
@@ -30170,13 +30233,13 @@
         <v>[User_login-131]</v>
       </c>
       <c r="B141" s="117" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C141" s="117" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D141" s="117" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E141" s="163"/>
       <c r="F141" s="117"/>
@@ -30191,13 +30254,13 @@
         <v>[User_login-132]</v>
       </c>
       <c r="B142" s="117" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C142" s="117" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D142" s="117" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E142" s="178"/>
       <c r="F142" s="117"/>
@@ -30272,7 +30335,7 @@
         <v>[User_login-137]</v>
       </c>
       <c r="B147" s="223" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C147" s="231"/>
       <c r="D147" s="231"/>
@@ -30289,13 +30352,13 @@
         <v>[User_login-138]</v>
       </c>
       <c r="B148" s="175" t="s">
+        <v>514</v>
+      </c>
+      <c r="C148" s="117" t="s">
+        <v>515</v>
+      </c>
+      <c r="D148" s="117" t="s">
         <v>516</v>
-      </c>
-      <c r="C148" s="117" t="s">
-        <v>517</v>
-      </c>
-      <c r="D148" s="117" t="s">
-        <v>518</v>
       </c>
       <c r="E148" s="163"/>
       <c r="F148" s="117"/>
@@ -30310,13 +30373,13 @@
         <v>[User_login-139]</v>
       </c>
       <c r="B149" s="175" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C149" s="117" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D149" s="117" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="E149" s="163"/>
       <c r="F149" s="117"/>
@@ -30331,13 +30394,13 @@
         <v>[User_login-140]</v>
       </c>
       <c r="B150" s="175" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C150" s="117" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D150" s="117" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="E150" s="163"/>
       <c r="F150" s="117"/>
@@ -30352,13 +30415,13 @@
         <v>[User_login-141]</v>
       </c>
       <c r="B151" s="175" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C151" s="117" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D151" s="117" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E151" s="163"/>
       <c r="F151" s="117"/>
@@ -30373,13 +30436,13 @@
         <v>[User_login-142]</v>
       </c>
       <c r="B152" s="175" t="s">
+        <v>523</v>
+      </c>
+      <c r="C152" s="117" t="s">
+        <v>524</v>
+      </c>
+      <c r="D152" s="117" t="s">
         <v>525</v>
-      </c>
-      <c r="C152" s="117" t="s">
-        <v>526</v>
-      </c>
-      <c r="D152" s="117" t="s">
-        <v>527</v>
       </c>
       <c r="E152" s="163"/>
       <c r="F152" s="117"/>
@@ -30394,7 +30457,7 @@
         <v>[User_login-143]</v>
       </c>
       <c r="B153" s="223" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C153" s="231"/>
       <c r="D153" s="231"/>
@@ -30411,13 +30474,13 @@
         <v>[User_login-144]</v>
       </c>
       <c r="B154" s="175" t="s">
+        <v>528</v>
+      </c>
+      <c r="C154" s="117" t="s">
+        <v>529</v>
+      </c>
+      <c r="D154" s="117" t="s">
         <v>530</v>
-      </c>
-      <c r="C154" s="117" t="s">
-        <v>531</v>
-      </c>
-      <c r="D154" s="117" t="s">
-        <v>532</v>
       </c>
       <c r="E154" s="118"/>
       <c r="F154" s="117"/>
@@ -30432,13 +30495,13 @@
         <v>[User_login-145]</v>
       </c>
       <c r="B155" s="175" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C155" s="117" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D155" s="117" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E155" s="118"/>
       <c r="F155" s="117"/>
@@ -30453,13 +30516,13 @@
         <v>[User_login-146]</v>
       </c>
       <c r="B156" s="175" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C156" s="117" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D156" s="117" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E156" s="118"/>
       <c r="F156" s="117"/>
@@ -30474,13 +30537,13 @@
         <v>[User_login-147]</v>
       </c>
       <c r="B157" s="175" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C157" s="117" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D157" s="117" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E157" s="118"/>
       <c r="F157" s="117"/>
@@ -30495,13 +30558,13 @@
         <v>[User_login-148]</v>
       </c>
       <c r="B158" s="175" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C158" s="117" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D158" s="117" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E158" s="118"/>
       <c r="F158" s="117"/>
@@ -30516,13 +30579,13 @@
         <v>[User_login-149]</v>
       </c>
       <c r="B159" s="243" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C159" s="117" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D159" s="117" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E159" s="118"/>
       <c r="F159" s="117"/>
@@ -30876,13 +30939,13 @@
         <v>ID-154</v>
       </c>
       <c r="B175" s="117" t="s">
+        <v>697</v>
+      </c>
+      <c r="C175" s="117" t="s">
+        <v>698</v>
+      </c>
+      <c r="D175" s="117" t="s">
         <v>699</v>
-      </c>
-      <c r="C175" s="117" t="s">
-        <v>700</v>
-      </c>
-      <c r="D175" s="117" t="s">
-        <v>701</v>
       </c>
       <c r="E175" s="117"/>
       <c r="F175" s="117"/>
@@ -31097,7 +31160,7 @@
   <dimension ref="A1:J80"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:G6"/>
+      <selection activeCell="G12" sqref="G12:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.25" defaultRowHeight="13.5" customHeight="1"/>
@@ -31302,8 +31365,12 @@
         <v>299</v>
       </c>
       <c r="E12" s="180"/>
-      <c r="F12" s="117"/>
-      <c r="G12" s="117"/>
+      <c r="F12" s="117" t="s">
+        <v>718</v>
+      </c>
+      <c r="G12" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H12" s="183"/>
       <c r="I12" s="181"/>
     </row>
@@ -31471,7 +31538,7 @@
     <row r="21" spans="1:10" ht="14.25" customHeight="1">
       <c r="A21" s="185"/>
       <c r="B21" s="186" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C21" s="185"/>
       <c r="D21" s="185"/>
@@ -31554,7 +31621,7 @@
     <row r="25" spans="1:10" ht="14.25" customHeight="1">
       <c r="A25" s="185"/>
       <c r="B25" s="186" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C25" s="185"/>
       <c r="D25" s="185"/>
@@ -31634,13 +31701,13 @@
         <v>[Admin_login-19]</v>
       </c>
       <c r="B29" s="117" t="s">
+        <v>573</v>
+      </c>
+      <c r="C29" s="117" t="s">
         <v>575</v>
       </c>
-      <c r="C29" s="117" t="s">
+      <c r="D29" s="189" t="s">
         <v>577</v>
-      </c>
-      <c r="D29" s="189" t="s">
-        <v>579</v>
       </c>
       <c r="E29" s="188"/>
       <c r="F29" s="117"/>
@@ -31655,13 +31722,13 @@
         <v>[Admin_login-20]</v>
       </c>
       <c r="B30" s="117" t="s">
+        <v>574</v>
+      </c>
+      <c r="C30" s="117" t="s">
         <v>576</v>
       </c>
-      <c r="C30" s="117" t="s">
+      <c r="D30" s="189" t="s">
         <v>578</v>
-      </c>
-      <c r="D30" s="189" t="s">
-        <v>580</v>
       </c>
       <c r="E30" s="188"/>
       <c r="F30" s="117"/>
@@ -31676,7 +31743,7 @@
         <v>[Admin_login-21]</v>
       </c>
       <c r="B31" s="186" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C31" s="185"/>
       <c r="D31" s="185"/>
@@ -31693,13 +31760,13 @@
         <v>[Admin_login-22]</v>
       </c>
       <c r="B32" s="117" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C32" s="117" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D32" s="189" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="E32" s="188"/>
       <c r="F32" s="117"/>
@@ -31714,13 +31781,13 @@
         <v>[Admin_login-23]</v>
       </c>
       <c r="B33" s="117" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C33" s="117" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D33" s="189" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E33" s="188"/>
       <c r="F33" s="117"/>
@@ -31735,13 +31802,13 @@
         <v>[Admin_login-24]</v>
       </c>
       <c r="B34" s="117" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C34" s="117" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D34" s="189" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="E34" s="188"/>
       <c r="F34" s="117"/>
@@ -31756,13 +31823,13 @@
         <v>[Admin_login-25]</v>
       </c>
       <c r="B35" s="117" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C35" s="117" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D35" s="189" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E35" s="188"/>
       <c r="F35" s="117"/>
@@ -31777,13 +31844,13 @@
         <v>[Admin_login-26]</v>
       </c>
       <c r="B36" s="117" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C36" s="117" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D36" s="189" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="E36" s="188"/>
       <c r="F36" s="117"/>
@@ -31798,13 +31865,13 @@
         <v>[Admin_login-27]</v>
       </c>
       <c r="B37" s="117" t="s">
+        <v>551</v>
+      </c>
+      <c r="C37" s="117" t="s">
+        <v>552</v>
+      </c>
+      <c r="D37" s="189" t="s">
         <v>553</v>
-      </c>
-      <c r="C37" s="117" t="s">
-        <v>554</v>
-      </c>
-      <c r="D37" s="189" t="s">
-        <v>555</v>
       </c>
       <c r="E37" s="188"/>
       <c r="F37" s="117"/>
@@ -31819,13 +31886,13 @@
         <v>[Admin_login-28]</v>
       </c>
       <c r="B38" s="117" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C38" s="117" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D38" s="189" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="E38" s="188"/>
       <c r="F38" s="117"/>
@@ -31840,13 +31907,13 @@
         <v>[Admin_login-29]</v>
       </c>
       <c r="B39" s="117" t="s">
+        <v>580</v>
+      </c>
+      <c r="C39" s="117" t="s">
+        <v>581</v>
+      </c>
+      <c r="D39" s="189" t="s">
         <v>582</v>
-      </c>
-      <c r="C39" s="117" t="s">
-        <v>583</v>
-      </c>
-      <c r="D39" s="189" t="s">
-        <v>584</v>
       </c>
       <c r="E39" s="188"/>
       <c r="F39" s="117"/>
@@ -31861,13 +31928,13 @@
         <v>[Admin_login-30]</v>
       </c>
       <c r="B40" s="117" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C40" s="117" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D40" s="189" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="E40" s="188"/>
       <c r="F40" s="117"/>
@@ -31882,7 +31949,7 @@
         <v>[Admin_login-31]</v>
       </c>
       <c r="B41" s="186" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C41" s="185"/>
       <c r="D41" s="185"/>
@@ -31899,13 +31966,13 @@
         <v>[Admin_login-32]</v>
       </c>
       <c r="B42" s="117" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C42" s="117" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D42" s="189" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E42" s="188"/>
       <c r="F42" s="117"/>
@@ -31920,13 +31987,13 @@
         <v>[Admin_login-33]</v>
       </c>
       <c r="B43" s="117" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C43" s="117" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D43" s="189" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="E43" s="188"/>
       <c r="F43" s="117"/>
@@ -31941,13 +32008,13 @@
         <v>[Admin_login-34]</v>
       </c>
       <c r="B44" s="117" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C44" s="117" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D44" s="189" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="E44" s="188"/>
       <c r="F44" s="117"/>
@@ -31962,13 +32029,13 @@
         <v>[Admin_login-35]</v>
       </c>
       <c r="B45" s="117" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C45" s="117" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D45" s="189" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E45" s="188"/>
       <c r="F45" s="117"/>
@@ -31983,13 +32050,13 @@
         <v>[Admin_login-36]</v>
       </c>
       <c r="B46" s="117" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C46" s="117" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D46" s="189" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E46" s="188"/>
       <c r="F46" s="117"/>
@@ -32004,13 +32071,13 @@
         <v>[Admin_login-37]</v>
       </c>
       <c r="B47" s="117" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C47" s="117" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D47" s="189" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="E47" s="188"/>
       <c r="F47" s="117"/>
@@ -32025,13 +32092,13 @@
         <v>[Admin_login-38]</v>
       </c>
       <c r="B48" s="117" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="C48" s="117" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D48" s="189" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E48" s="188"/>
       <c r="F48" s="188"/>
@@ -32046,13 +32113,13 @@
         <v>[Admin_login-39]</v>
       </c>
       <c r="B49" s="117" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C49" s="117" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D49" s="189" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E49" s="188"/>
       <c r="F49" s="188"/>
@@ -32067,13 +32134,13 @@
         <v>[Admin_login-40]</v>
       </c>
       <c r="B50" s="117" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C50" s="117" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D50" s="189" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="E50" s="188"/>
       <c r="F50" s="117"/>
@@ -32088,13 +32155,13 @@
         <v>[Admin_login-41]</v>
       </c>
       <c r="B51" s="117" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C51" s="117" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D51" s="189" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E51" s="188"/>
       <c r="F51" s="117"/>
@@ -32109,13 +32176,13 @@
         <v>[Admin_login-42]</v>
       </c>
       <c r="B52" s="117" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C52" s="117" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="D52" s="189" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="E52" s="188"/>
       <c r="F52" s="117"/>
@@ -32127,7 +32194,7 @@
     <row r="53" spans="1:10" ht="14.25" customHeight="1">
       <c r="A53" s="165"/>
       <c r="B53" s="186" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C53" s="185"/>
       <c r="D53" s="185"/>
@@ -32144,13 +32211,13 @@
         <v>[Admin_login-44]</v>
       </c>
       <c r="B54" s="117" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="C54" s="117" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D54" s="189" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="E54" s="188"/>
       <c r="F54" s="117"/>
@@ -32165,13 +32232,13 @@
         <v>[Admin_login-45]</v>
       </c>
       <c r="B55" s="117" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C55" s="117" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D55" s="189" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E55" s="188"/>
       <c r="F55" s="117"/>
@@ -32186,13 +32253,13 @@
         <v>[Admin_login-46]</v>
       </c>
       <c r="B56" s="117" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C56" s="117" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D56" s="189" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="E56" s="188"/>
       <c r="F56" s="117"/>
@@ -32207,13 +32274,13 @@
         <v>[Admin_login-47]</v>
       </c>
       <c r="B57" s="117" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C57" s="117" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D57" s="189" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="E57" s="188"/>
       <c r="F57" s="117"/>
@@ -32228,13 +32295,13 @@
         <v>[Admin_login-48]</v>
       </c>
       <c r="B58" s="117" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C58" s="117" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D58" s="189" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="E58" s="188"/>
       <c r="F58" s="117"/>
@@ -32249,13 +32316,13 @@
         <v>[Admin_login-49]</v>
       </c>
       <c r="B59" s="117" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C59" s="117" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D59" s="189" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="E59" s="188"/>
       <c r="F59" s="117"/>
@@ -32270,13 +32337,13 @@
         <v>[Admin_login-50]</v>
       </c>
       <c r="B60" s="117" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C60" s="117" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="D60" s="189" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="E60" s="188"/>
       <c r="F60" s="117"/>
@@ -32291,13 +32358,13 @@
         <v>[Admin_login-51]</v>
       </c>
       <c r="B61" s="117" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="C61" s="117" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="D61" s="189" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="E61" s="188"/>
       <c r="F61" s="117"/>
@@ -32312,13 +32379,13 @@
         <v>[Admin_login-52]</v>
       </c>
       <c r="B62" s="117" t="s">
+        <v>614</v>
+      </c>
+      <c r="C62" s="117" t="s">
         <v>616</v>
       </c>
-      <c r="C62" s="117" t="s">
-        <v>618</v>
-      </c>
       <c r="D62" s="189" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="E62" s="188"/>
       <c r="F62" s="117"/>
@@ -32333,13 +32400,13 @@
         <v>[Admin_login-53]</v>
       </c>
       <c r="B63" s="117" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="C63" s="117" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D63" s="189" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="E63" s="188"/>
       <c r="F63" s="117"/>
@@ -32354,13 +32421,13 @@
         <v>[Admin_login-54]</v>
       </c>
       <c r="B64" s="117" t="s">
+        <v>622</v>
+      </c>
+      <c r="C64" s="117" t="s">
+        <v>623</v>
+      </c>
+      <c r="D64" s="189" t="s">
         <v>624</v>
-      </c>
-      <c r="C64" s="117" t="s">
-        <v>625</v>
-      </c>
-      <c r="D64" s="189" t="s">
-        <v>626</v>
       </c>
       <c r="E64" s="188"/>
       <c r="F64" s="117"/>
@@ -32375,13 +32442,13 @@
         <v>[Admin_login-55]</v>
       </c>
       <c r="B65" s="117" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C65" s="117" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="D65" s="189" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="E65" s="168"/>
       <c r="F65" s="117"/>
@@ -32396,13 +32463,13 @@
         <v>[Admin_login-56]</v>
       </c>
       <c r="B66" s="117" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C66" s="117" t="s">
+        <v>625</v>
+      </c>
+      <c r="D66" s="189" t="s">
         <v>627</v>
-      </c>
-      <c r="D66" s="189" t="s">
-        <v>629</v>
       </c>
       <c r="E66" s="168"/>
       <c r="F66" s="117"/>
@@ -32417,13 +32484,13 @@
         <v>[Admin_login-57]</v>
       </c>
       <c r="B67" s="117" t="s">
+        <v>630</v>
+      </c>
+      <c r="C67" s="117" t="s">
+        <v>631</v>
+      </c>
+      <c r="D67" s="189" t="s">
         <v>632</v>
-      </c>
-      <c r="C67" s="117" t="s">
-        <v>633</v>
-      </c>
-      <c r="D67" s="189" t="s">
-        <v>634</v>
       </c>
       <c r="E67" s="168"/>
       <c r="F67" s="117"/>
@@ -32438,13 +32505,13 @@
         <v>[Admin_login-58]</v>
       </c>
       <c r="B68" s="117" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C68" s="117" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D68" s="189" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E68" s="168"/>
       <c r="F68" s="117"/>
@@ -32459,13 +32526,13 @@
         <v>[Admin_login-59]</v>
       </c>
       <c r="B69" s="117" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C69" s="117" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="D69" s="189" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="E69" s="168"/>
       <c r="F69" s="117"/>
@@ -32480,13 +32547,13 @@
         <v>[Admin_login-60]</v>
       </c>
       <c r="B70" s="117" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="C70" s="117" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="D70" s="189" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="E70" s="168"/>
       <c r="F70" s="117"/>
@@ -32501,13 +32568,13 @@
         <v>[Admin_login-61]</v>
       </c>
       <c r="B71" s="117" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C71" s="117" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="D71" s="189" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="E71" s="168"/>
       <c r="F71" s="117"/>
@@ -32522,13 +32589,13 @@
         <v>[Admin_login-62]</v>
       </c>
       <c r="B72" s="117" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C72" s="117" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D72" s="189" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="E72" s="168"/>
       <c r="F72" s="117"/>
@@ -32543,13 +32610,13 @@
         <v>[Admin_login-63]</v>
       </c>
       <c r="B73" s="117" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C73" s="117" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D73" s="189" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="E73" s="168"/>
       <c r="F73" s="117"/>
@@ -32564,13 +32631,13 @@
         <v>[Admin_login-64]</v>
       </c>
       <c r="B74" s="117" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C74" s="117" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D74" s="189" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="E74" s="168"/>
       <c r="F74" s="117"/>
@@ -32585,13 +32652,13 @@
         <v>[Admin_login-65]</v>
       </c>
       <c r="B75" s="117" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C75" s="117" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="D75" s="189" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="E75" s="168"/>
       <c r="F75" s="117"/>
@@ -32606,13 +32673,13 @@
         <v>[Admin_login-66]</v>
       </c>
       <c r="B76" s="117" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="C76" s="117" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="D76" s="189" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="E76" s="168"/>
       <c r="F76" s="117"/>
@@ -32627,13 +32694,13 @@
         <v>[Admin_login-67]</v>
       </c>
       <c r="B77" s="117" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C77" s="117" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="D77" s="189" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="E77" s="168"/>
       <c r="F77" s="117"/>
@@ -32648,13 +32715,13 @@
         <v>[Admin_login-68]</v>
       </c>
       <c r="B78" s="117" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C78" s="117" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="D78" s="189" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="E78" s="168"/>
       <c r="F78" s="117"/>
@@ -32669,13 +32736,13 @@
         <v>[Admin_login-69]</v>
       </c>
       <c r="B79" s="117" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C79" s="117" t="s">
+        <v>660</v>
+      </c>
+      <c r="D79" s="189" t="s">
         <v>662</v>
-      </c>
-      <c r="D79" s="189" t="s">
-        <v>664</v>
       </c>
       <c r="E79" s="168"/>
       <c r="F79" s="117"/>
@@ -32690,13 +32757,13 @@
         <v>[Admin_login-70]</v>
       </c>
       <c r="B80" s="117" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C80" s="117" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="D80" s="189" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="E80" s="168"/>
       <c r="F80" s="117"/>
@@ -32714,12 +32781,15 @@
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="E6:G6"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G8">
       <formula1>$H$2:$H$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G1:G3 F26:G26 F32:G40 F42:G48 F50:G52 F22:G24 F12:G20 F28:G30 F54:G80">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G1:G3 F26:G26 F32:G40 F42:G48 F50:G52 F22:G24 F54:G80 F28:G30 G12:G20 F13:F20">
       <formula1>$J$2:$J$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F12">
+      <formula1>TestList</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -32729,4 +32799,39 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>